<commit_message>
Edited the Meng Report
</commit_message>
<xml_diff>
--- a/MEng_TaskB/Adult/classification_model_results.xlsx
+++ b/MEng_TaskB/Adult/classification_model_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabel/SUN/03_DataScience/00_PostBlock/PBA3_19May/ds-group-42-pba-3/MEng_TaskB/Adult/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18282275-6291-304C-B0FD-273DA7BC0702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA19AE6-CBE7-164D-A525-2F15055C3810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="1760" windowWidth="25660" windowHeight="10580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,6 +74,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -420,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -452,162 +453,162 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2">
-        <v>0.80663322755655642</v>
+        <v>0.81113727095915655</v>
       </c>
       <c r="D2">
-        <v>0.79114315683906911</v>
+        <v>0.79614872458487684</v>
       </c>
       <c r="E2">
-        <v>0.80663322755655642</v>
+        <v>0.81113727095915655</v>
       </c>
       <c r="F2">
-        <v>0.79250085765419731</v>
+        <v>0.78879480622315157</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3">
-        <v>0.70907974204115054</v>
+        <v>0.76998669259903774</v>
       </c>
       <c r="D3">
-        <v>0.74608020309512013</v>
+        <v>0.77376309992929382</v>
       </c>
       <c r="E3">
-        <v>0.70907974204115054</v>
+        <v>0.76998669259903774</v>
       </c>
       <c r="F3">
-        <v>0.72264749886069268</v>
+        <v>0.77177381193877159</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4">
-        <v>0.56658818712253045</v>
+        <v>0.80663322755655642</v>
       </c>
       <c r="D4">
-        <v>0.75494946409264829</v>
+        <v>0.79114315683906911</v>
       </c>
       <c r="E4">
-        <v>0.56658818712253045</v>
+        <v>0.80663322755655642</v>
       </c>
       <c r="F4">
-        <v>0.59484576263802624</v>
+        <v>0.79250085765419731</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5">
-        <v>0.54611526256525744</v>
+        <v>0.70907974204115054</v>
       </c>
       <c r="D5">
-        <v>0.72284536196831894</v>
+        <v>0.74608020309512013</v>
       </c>
       <c r="E5">
-        <v>0.54611526256525744</v>
+        <v>0.70907974204115054</v>
       </c>
       <c r="F5">
-        <v>0.57673703679745625</v>
+        <v>0.72264749886069268</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6">
-        <v>0.26164397584194898</v>
+        <v>0.56658818712253045</v>
       </c>
       <c r="D6">
-        <v>0.72185401505440516</v>
+        <v>0.75494946409264829</v>
       </c>
       <c r="E6">
-        <v>0.26164397584194898</v>
+        <v>0.56658818712253045</v>
       </c>
       <c r="F6">
-        <v>0.14568881689230639</v>
+        <v>0.59484576263802624</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7">
-        <v>0.39082812979834169</v>
+        <v>0.54611526256525744</v>
       </c>
       <c r="D7">
-        <v>0.68432286173780987</v>
+        <v>0.72284536196831894</v>
       </c>
       <c r="E7">
-        <v>0.39082812979834169</v>
+        <v>0.54611526256525744</v>
       </c>
       <c r="F7">
-        <v>0.39160898070338468</v>
+        <v>0.57673703679745625</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8">
-        <v>0.81113727095915655</v>
+        <v>0.26164397584194898</v>
       </c>
       <c r="D8">
-        <v>0.79614872458487684</v>
+        <v>0.72185401505440516</v>
       </c>
       <c r="E8">
-        <v>0.81113727095915655</v>
+        <v>0.26164397584194898</v>
       </c>
       <c r="F8">
-        <v>0.78879480622315157</v>
+        <v>0.14568881689230639</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9">
-        <v>0.76998669259903774</v>
+        <v>0.39082812979834169</v>
       </c>
       <c r="D9">
-        <v>0.77376309992929382</v>
+        <v>0.68432286173780987</v>
       </c>
       <c r="E9">
-        <v>0.76998669259903774</v>
+        <v>0.39082812979834169</v>
       </c>
       <c r="F9">
-        <v>0.77177381193877159</v>
+        <v>0.39160898070338468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on the report and visualisations
</commit_message>
<xml_diff>
--- a/MEng_TaskB/Adult/classification_model_results.xlsx
+++ b/MEng_TaskB/Adult/classification_model_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabel/SUN/03_DataScience/00_PostBlock/PBA3_19May/ds-group-42-pba-3/MEng_TaskB/Adult/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2D02CE-5D42-9446-BF52-F8CB55034D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BFEF04-9B85-6145-B571-505198E4BCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="k-NN" sheetId="1" r:id="rId1"/>
@@ -22,15 +22,6 @@
     <sheet name="NewResults_Graphs" sheetId="10" r:id="rId7"/>
     <sheet name="NewResults_End)" sheetId="11" r:id="rId8"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'NewResults_End)'!$A$27:$A$29</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'NewResults_End)'!$B$26</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'NewResults_End)'!$B$27:$B$29</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'NewResults_End)'!$C$26</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'NewResults_End)'!$C$27:$C$29</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'NewResults_End)'!$D$26</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'NewResults_End)'!$D$27:$D$29</definedName>
-  </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -49,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="30">
   <si>
     <t>dataset_name</t>
   </si>
@@ -121,6 +112,24 @@
   </si>
   <si>
     <t>Control</t>
+  </si>
+  <si>
+    <t>Control(Accuracy)</t>
+  </si>
+  <si>
+    <t>Mean(Accuracy)</t>
+  </si>
+  <si>
+    <t>k-NN(Accuracy)</t>
+  </si>
+  <si>
+    <t>Control(F1)</t>
+  </si>
+  <si>
+    <t>Mean(F1)</t>
+  </si>
+  <si>
+    <t>k-NN(F1)</t>
   </si>
 </sst>
 </file>
@@ -230,7 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -258,16 +267,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4735,7 +4743,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Control</c:v>
+                  <c:v>Control(Accuracy)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4801,7 +4809,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Mean</c:v>
+                  <c:v>Mean(Accuracy)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4867,7 +4875,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>k-NN</c:v>
+                  <c:v>k-NN(Accuracy)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5759,7 +5767,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Control</c:v>
+                  <c:v>Control(Accuracy)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5825,7 +5833,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Mean</c:v>
+                  <c:v>Mean(Accuracy)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5891,7 +5899,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>k-NN</c:v>
+                  <c:v>k-NN(Accuracy)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6350,7 +6358,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Control</c:v>
+                  <c:v>Control(F1)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6416,7 +6424,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Mean</c:v>
+                  <c:v>Mean(F1)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6482,7 +6490,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>k-NN</c:v>
+                  <c:v>k-NN(F1)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6703,7 +6711,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> Accuracy</a:t>
+                  <a:t> F1</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -6941,7 +6949,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Control</c:v>
+                  <c:v>Control(F1)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7007,7 +7015,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Mean</c:v>
+                  <c:v>Mean(F1)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7073,7 +7081,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>k-NN</c:v>
+                  <c:v>k-NN(F1)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7294,7 +7302,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> Accuracy</a:t>
+                  <a:t> F1</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -7429,6 +7437,1411 @@
     </a:ln>
     <a:effectLst/>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Classification Tree: Performance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NewResults_End)'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Control(Accuracy)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$A$4:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$B$4:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.81113727095915655</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.81113727095915655</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.81113727095915655</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-6F6E-5449-AFCC-88C437AA697E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NewResults_End)'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean(Accuracy)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$A$4:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$C$4:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.8123656464325929</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78104207185996521</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.76292353362677856</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-6F6E-5449-AFCC-88C437AA697E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NewResults_End)'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>k-NN(Accuracy)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$A$4:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$D$4:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.80663300000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56658799999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26164399999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-6F6E-5449-AFCC-88C437AA697E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NewResults_End)'!$N$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Control(F1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$A$4:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$N$4:$N$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.78879480622315157</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78879480622315157</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78879480622315157</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-6F6E-5449-AFCC-88C437AA697E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NewResults_End)'!$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean(F1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$A$4:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$O$4:$O$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.78560311502942748</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71767430595285797</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.661535050357556</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-6F6E-5449-AFCC-88C437AA697E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NewResults_End)'!$P$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>k-NN(F1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$A$4:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$P$4:$P$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.79250100000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.59484599999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14568900000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-6F6E-5449-AFCC-88C437AA697E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="397713664"/>
+        <c:axId val="397715392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="397713664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Proportion of Missing Values Imputed</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397715392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="397715392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Performance metric score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397713664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>k-Nerest Neighbour Performance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NewResults_End)'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Control(Accuracy)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$A$27:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$B$27:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.80745214453884695</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.80745214453884695</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.80745214453884695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-AB5A-AD40-BE72-FB4A83BC126D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NewResults_End)'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean(Accuracy)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$A$27:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$C$27:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.78513665677141975</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77459310062442421</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.74961613266455118</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-AB5A-AD40-BE72-FB4A83BC126D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NewResults_End)'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>k-NN(Accuracy)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$A$27:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$D$27:$D$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.78431799999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.61203799999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.31958199999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-AB5A-AD40-BE72-FB4A83BC126D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NewResults_End)'!$N$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Control(F1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$A$27:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$N$27:$N$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.80039686949754418</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.80039686949754418</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.80039686949754418</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-AB5A-AD40-BE72-FB4A83BC126D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NewResults_End)'!$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean(F1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$A$27:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$O$27:$O$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.77208995728365548</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.74705270822564263</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.71571575033308343</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-AB5A-AD40-BE72-FB4A83BC126D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'NewResults_End)'!$P$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>k-NN(F1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$A$27:$A$29</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'NewResults_End)'!$P$27:$P$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.78365399999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.64047299999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26821</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-AB5A-AD40-BE72-FB4A83BC126D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="397713664"/>
+        <c:axId val="397715392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="397713664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Proportion of Missing Values Imputed</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397715392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="397715392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Performance metric score</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="397713664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -23413,10 +24826,10 @@
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28222</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23451,8 +24864,8 @@
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>197556</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:to>
@@ -23483,16 +24896,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>155222</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23521,15 +24934,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>536224</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>197555</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>536224</xdr:colOff>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -23557,13 +24970,89 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>691445</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>520701</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A14DE6F8-1AA0-B042-BB66-BE6FF4490FA8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>155222</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>98777</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43732A10-93FC-8E4E-A4B4-CDB46C410031}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Blue Warm">
+    <a:clrScheme name="Blue">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -23571,34 +25060,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="242852"/>
+        <a:srgbClr val="17406D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ACCBF9"/>
+        <a:srgbClr val="DBEFF9"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4A66AC"/>
+        <a:srgbClr val="0F6FC6"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="629DD1"/>
+        <a:srgbClr val="009DD9"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="297FD5"/>
+        <a:srgbClr val="0BD0D9"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="7F8FA9"/>
+        <a:srgbClr val="10CF9B"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5AA2AE"/>
+        <a:srgbClr val="7CCA62"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="9D90A0"/>
+        <a:srgbClr val="A5C249"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="9454C3"/>
+        <a:srgbClr val="F49100"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="3EBBF0"/>
+        <a:srgbClr val="85DFD0"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -25080,35 +26569,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="16"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
@@ -25277,35 +26766,35 @@
       <c r="K11" s="5"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16" t="s">
+      <c r="C26" s="19"/>
+      <c r="D26" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16" t="s">
+      <c r="E26" s="19"/>
+      <c r="F26" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16" t="s">
+      <c r="G26" s="19"/>
+      <c r="H26" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I26" s="16"/>
+      <c r="I26" s="19"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
@@ -25451,16 +26940,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A25:I25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A25:I25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -25681,7 +27170,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:I12"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25912,40 +27401,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="17"/>
+      <c r="D2" s="20"/>
       <c r="E2" s="13"/>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17" t="s">
+      <c r="G2" s="20"/>
+      <c r="H2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17" t="s">
+      <c r="I2" s="20"/>
+      <c r="J2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="17"/>
+      <c r="K2" s="20"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="14"/>
@@ -26124,40 +27613,40 @@
       <c r="M11" s="5"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="17"/>
+      <c r="D26" s="20"/>
       <c r="E26" s="13"/>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17" t="s">
+      <c r="G26" s="20"/>
+      <c r="H26" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17" t="s">
+      <c r="I26" s="20"/>
+      <c r="J26" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="K26" s="17"/>
+      <c r="K26" s="20"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="14"/>
@@ -26334,8 +27823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF06522-7AD8-8F4F-B195-C56521A4F0C4}">
   <dimension ref="A1:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="O51" sqref="O51"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AB38" sqref="AB38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -26357,62 +27846,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
-      <c r="G2" s="17" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="16"/>
+      <c r="G2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="17"/>
+      <c r="H2" s="20"/>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="17"/>
+      <c r="L2" s="20"/>
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="17"/>
+      <c r="P2" s="20"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="14"/>
       <c r="B3" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="19"/>
+        <v>26</v>
+      </c>
       <c r="F3" s="14" t="s">
         <v>23</v>
       </c>
@@ -26434,17 +27922,17 @@
       </c>
       <c r="M3" s="14"/>
       <c r="N3" s="14" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" s="20">
+      <c r="A4" s="17">
         <v>0.1</v>
       </c>
       <c r="B4" s="15">
@@ -26488,7 +27976,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="20">
+      <c r="A5" s="17">
         <v>0.4</v>
       </c>
       <c r="B5" s="15">
@@ -26532,7 +28020,7 @@
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" s="20">
+      <c r="A6" s="17">
         <v>0.7</v>
       </c>
       <c r="B6" s="15">
@@ -26598,63 +28086,62 @@
       <c r="R10" s="5"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="20"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="17"/>
+      <c r="D25" s="20"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
-      <c r="G25" s="17" t="s">
+      <c r="G25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H25" s="17"/>
+      <c r="H25" s="20"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
-      <c r="K25" s="17" t="s">
+      <c r="K25" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="L25" s="17"/>
+      <c r="L25" s="20"/>
       <c r="M25" s="13"/>
       <c r="N25" s="13"/>
-      <c r="O25" s="17" t="s">
+      <c r="O25" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="P25" s="17"/>
+      <c r="P25" s="20"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="14"/>
       <c r="B26" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="14"/>
+        <v>26</v>
+      </c>
       <c r="F26" s="14" t="s">
         <v>23</v>
       </c>
@@ -26676,17 +28163,17 @@
       </c>
       <c r="M26" s="14"/>
       <c r="N26" s="14" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="O26" s="14" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="P26" s="14" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="20">
+      <c r="A27" s="17">
         <v>0.1</v>
       </c>
       <c r="B27" s="15">
@@ -26730,7 +28217,7 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" s="20">
+      <c r="A28" s="17">
         <v>0.4</v>
       </c>
       <c r="B28" s="15">
@@ -26774,7 +28261,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="20">
+      <c r="A29" s="17">
         <v>0.7</v>
       </c>
       <c r="B29" s="15">
@@ -26818,7 +28305,7 @@
       </c>
     </row>
     <row r="34" spans="15:15" ht="19" x14ac:dyDescent="0.2">
-      <c r="O34" s="21"/>
+      <c r="O34" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>